<commit_message>
added data-info to get price and gallery
</commit_message>
<xml_diff>
--- a/dataset/data-infos.xlsx
+++ b/dataset/data-infos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c4b1d2011ae4f894/Documents/GitHub/order_experiment/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:40009_{9D7C50B8-D3FB-4B8D-8E37-DD15650E8EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD614077-0398-466A-A2E3-17300D06D2E4}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:40009_{9D7C50B8-D3FB-4B8D-8E37-DD15650E8EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B0E5920-2EAC-40E4-A9BD-EE404DD7C565}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2925" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="118">
   <si>
     <t>https://opensea.io/assets/ethereum/0xcb1021080b61dac7032618de925a62176cbc8372/2547</t>
   </si>
@@ -320,6 +320,60 @@
   </si>
   <si>
     <t>https://opensea.io/assets/ethereum/0x495f947276749ce646f68ac8c248420045cb7b5e/55009236754177688704712285819362994549214138196257374091251074634409597468673</t>
+  </si>
+  <si>
+    <t>KPR</t>
+  </si>
+  <si>
+    <t>WMN</t>
+  </si>
+  <si>
+    <t>BST</t>
+  </si>
+  <si>
+    <t>WHR</t>
+  </si>
+  <si>
+    <t>THM</t>
+  </si>
+  <si>
+    <t>GRN</t>
+  </si>
+  <si>
+    <t>JST</t>
+  </si>
+  <si>
+    <t>PLT</t>
+  </si>
+  <si>
+    <t>CLR</t>
+  </si>
+  <si>
+    <t>BTF</t>
+  </si>
+  <si>
+    <t>TYL</t>
+  </si>
+  <si>
+    <t>DSR</t>
+  </si>
+  <si>
+    <t>SPR</t>
+  </si>
+  <si>
+    <t>Picture Series</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Gallery</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -1319,1445 +1373,1762 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0.2</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0.17</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0.14990000000000001</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>0.129</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.14990000000000001</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0.129</v>
+      </c>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>0.12</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>3.1</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>1</v>
       </c>
       <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>3.1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C7">
-        <v>1.99</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1.99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C8">
-        <v>1.111</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>1</v>
       </c>
       <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>1.111</v>
+      </c>
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C9">
-        <v>0.9</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1</v>
       </c>
       <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>0.9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C10">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
         <v>0.75</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>2</v>
       </c>
       <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="C12">
-        <v>0.5</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>2</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>0.38</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>0.2</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2</v>
       </c>
       <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>0.2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>2</v>
+      </c>
+      <c r="B16">
         <v>4</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>0.78</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>3</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>75</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>3</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>3</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>3</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <v>28.75</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>3</v>
       </c>
       <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>28.75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>3</v>
+      </c>
+      <c r="B21">
         <v>4</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>15</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>1.2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>4</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>4</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>4</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>4</v>
       </c>
       <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>0.5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
         <v>4</v>
       </c>
-      <c r="C25">
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
         <v>0.42070000000000002</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="6">
-        <v>5</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>5</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>5</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>0.99</v>
+        <v>1.2</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>5</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>0.69</v>
+        <v>0.99</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>5</v>
       </c>
       <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>0.69</v>
+      </c>
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>5</v>
+      </c>
+      <c r="B31">
         <v>4</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>0.25</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="7">
-        <v>6</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>6</v>
       </c>
       <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
         <v>1</v>
       </c>
-      <c r="C32">
-        <v>0.8</v>
-      </c>
       <c r="D32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>6</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>0.68</v>
+        <v>0.8</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>6</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="D34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="E34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>6</v>
       </c>
       <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>0.5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>6</v>
+      </c>
+      <c r="B36">
         <v>4</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>0.34899999999999998</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="8">
-        <v>7</v>
-      </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <v>2.5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>7</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>7</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>1.65</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D38" t="s">
+        <v>101</v>
+      </c>
+      <c r="E38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>7</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>1.25</v>
+        <v>1.65</v>
       </c>
       <c r="D39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>7</v>
       </c>
       <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>1.25</v>
+      </c>
+      <c r="D40" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
+        <v>7</v>
+      </c>
+      <c r="B41">
         <v>4</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>0.98</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D41" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="9">
-        <v>8</v>
-      </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41">
-        <v>130</v>
-      </c>
-      <c r="D41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="9">
         <v>8</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="E42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="9">
         <v>8</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="D43" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="E43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
         <v>8</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="D44" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="E44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="9">
         <v>8</v>
       </c>
       <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>49</v>
+      </c>
+      <c r="D45" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="9">
+        <v>8</v>
+      </c>
+      <c r="B46">
         <v>4</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>30</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="10">
-        <v>9</v>
-      </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>100</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="10">
         <v>9</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <v>85.69</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D47" t="s">
+        <v>106</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="10">
         <v>9</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <v>55</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>85.69</v>
+      </c>
+      <c r="D48" t="s">
+        <v>106</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="10">
         <v>9</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49">
-        <v>40.665999999999997</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="D49" t="s">
+        <v>106</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="10">
         <v>9</v>
       </c>
       <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>40.665999999999997</v>
+      </c>
+      <c r="D50" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="10">
+        <v>9</v>
+      </c>
+      <c r="B51">
         <v>4</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>4.5</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D51" t="s">
+        <v>106</v>
+      </c>
+      <c r="E51" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="13">
-        <v>10</v>
-      </c>
-      <c r="B51">
-        <v>0</v>
-      </c>
-      <c r="C51">
-        <v>1.38</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="13">
         <v>10</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52">
-        <v>0.5</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.38</v>
+      </c>
+      <c r="D52" t="s">
+        <v>107</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>10</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53">
-        <v>0.39</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>107</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="13">
         <v>10</v>
       </c>
       <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="C54" s="12">
-        <v>0.32</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C54">
+        <v>0.39</v>
+      </c>
+      <c r="D54" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="13">
         <v>10</v>
       </c>
       <c r="B55">
+        <v>3</v>
+      </c>
+      <c r="C55" s="12">
+        <v>0.32</v>
+      </c>
+      <c r="D55" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="13">
+        <v>10</v>
+      </c>
+      <c r="B56">
         <v>4</v>
       </c>
-      <c r="C55">
+      <c r="C56">
         <v>0.3</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D56" t="s">
+        <v>107</v>
+      </c>
+      <c r="E56" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="14">
-        <v>11</v>
-      </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
-      <c r="C56">
-        <v>0.37</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
         <v>11</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57">
-        <v>0.29499999999999998</v>
+        <v>0.37</v>
       </c>
       <c r="D57" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
         <v>11</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>0.25</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="D58" t="s">
+        <v>108</v>
+      </c>
+      <c r="E58" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="14">
         <v>11</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="D59" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="14">
         <v>11</v>
       </c>
       <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <v>0.15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>108</v>
+      </c>
+      <c r="E60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="14">
+        <v>11</v>
+      </c>
+      <c r="B61">
         <v>4</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>0.12</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
+        <v>108</v>
+      </c>
+      <c r="E61" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="15">
-        <v>12</v>
-      </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="C61">
-        <v>0.48</v>
-      </c>
-      <c r="D61" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <v>12</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62">
-        <v>0.41899999999999998</v>
+        <v>0.48</v>
       </c>
       <c r="D62" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="E62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="15">
         <v>12</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C63">
-        <v>0.33900000000000002</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="D63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="E63" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="15">
         <v>12</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C64">
-        <v>0.25</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="D64" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <v>12</v>
       </c>
       <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <v>0.25</v>
+      </c>
+      <c r="D65" t="s">
+        <v>104</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="15">
+        <v>12</v>
+      </c>
+      <c r="B66">
         <v>4</v>
       </c>
-      <c r="C65">
+      <c r="C66">
         <v>0.2</v>
       </c>
-      <c r="D65" s="11" t="s">
+      <c r="D66" t="s">
+        <v>104</v>
+      </c>
+      <c r="E66" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="16">
-        <v>13</v>
-      </c>
-      <c r="B66">
-        <v>0</v>
-      </c>
-      <c r="C66">
-        <v>0.05</v>
-      </c>
-      <c r="D66" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="16">
         <v>13</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C67">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="D67" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="E67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="16">
         <v>13</v>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C68">
-        <v>0.32</v>
+        <v>0.04</v>
       </c>
       <c r="D68" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="E68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="16">
         <v>13</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C69">
-        <v>2.8000000000000001E-2</v>
+        <v>0.32</v>
       </c>
       <c r="D69" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="E69" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="16">
         <v>13</v>
       </c>
       <c r="B70">
+        <v>3</v>
+      </c>
+      <c r="C70">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>109</v>
+      </c>
+      <c r="E70" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="16">
+        <v>13</v>
+      </c>
+      <c r="B71">
         <v>4</v>
       </c>
-      <c r="C70">
+      <c r="C71">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
+        <v>109</v>
+      </c>
+      <c r="E71" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="17">
-        <v>14</v>
-      </c>
-      <c r="B71">
-        <v>0</v>
-      </c>
-      <c r="C71">
-        <v>70</v>
-      </c>
-      <c r="D71" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="17">
         <v>14</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C72">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D72" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="E72" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="17">
         <v>14</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C73">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D73" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="E73" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="17">
         <v>14</v>
       </c>
       <c r="B74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C74">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D74" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="E74" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="17">
         <v>14</v>
       </c>
       <c r="B75">
+        <v>3</v>
+      </c>
+      <c r="C75">
+        <v>40</v>
+      </c>
+      <c r="D75" t="s">
+        <v>103</v>
+      </c>
+      <c r="E75" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="17">
+        <v>14</v>
+      </c>
+      <c r="B76">
         <v>4</v>
       </c>
-      <c r="C75">
+      <c r="C76">
         <v>29.37</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
+        <v>103</v>
+      </c>
+      <c r="E76" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="18">
-        <v>15</v>
-      </c>
-      <c r="B76">
-        <v>0</v>
-      </c>
-      <c r="C76">
-        <v>0.1</v>
-      </c>
-      <c r="D76" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="18">
         <v>15</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77">
         <v>0.1</v>
       </c>
       <c r="D77" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="E77" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="18">
         <v>15</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78">
         <v>0.1</v>
       </c>
       <c r="D78" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="E78" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="18">
         <v>15</v>
       </c>
       <c r="B79">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C79">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="D79" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="E79" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="18">
         <v>15</v>
       </c>
       <c r="B80">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C80">
         <v>0.9</v>
       </c>
       <c r="D80" t="s">
+        <v>110</v>
+      </c>
+      <c r="E80" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="18">
+        <v>15</v>
+      </c>
+      <c r="B81">
+        <v>4</v>
+      </c>
+      <c r="C81">
+        <v>0.9</v>
+      </c>
+      <c r="D81" t="s">
+        <v>110</v>
+      </c>
+      <c r="E81" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="19">
-        <v>16</v>
-      </c>
-      <c r="B81">
-        <v>0</v>
-      </c>
-      <c r="C81">
-        <v>0.25</v>
-      </c>
-      <c r="D81" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="19">
         <v>16</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82">
         <v>0.25</v>
       </c>
       <c r="D82" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="E82" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="19">
         <v>16</v>
       </c>
       <c r="B83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C83">
         <v>0.25</v>
       </c>
       <c r="D83" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="E83" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="19">
         <v>16</v>
       </c>
       <c r="B84">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C84">
         <v>0.25</v>
       </c>
-      <c r="D84" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
+        <v>111</v>
+      </c>
+      <c r="E84" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="19">
         <v>16</v>
       </c>
       <c r="B85">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C85">
         <v>0.25</v>
       </c>
       <c r="D85" t="s">
+        <v>111</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="19">
+        <v>16</v>
+      </c>
+      <c r="B86">
+        <v>4</v>
+      </c>
+      <c r="C86">
+        <v>0.25</v>
+      </c>
+      <c r="D86" t="s">
+        <v>111</v>
+      </c>
+      <c r="E86" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="20">
-        <v>17</v>
-      </c>
-      <c r="B86">
-        <v>0</v>
-      </c>
-      <c r="C86">
-        <v>0.21</v>
-      </c>
-      <c r="D86" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="20">
         <v>17</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87">
         <v>0.21</v>
       </c>
-      <c r="D87" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D87" t="s">
+        <v>111</v>
+      </c>
+      <c r="E87" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="20">
         <v>17</v>
       </c>
       <c r="B88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C88">
         <v>0.21</v>
       </c>
       <c r="D88" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="20">
         <v>17</v>
       </c>
       <c r="B89">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="D89" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="E89" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="20">
         <v>17</v>
       </c>
       <c r="B90">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C90">
         <v>0.2</v>
       </c>
       <c r="D90" t="s">
+        <v>111</v>
+      </c>
+      <c r="E90" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="20">
+        <v>17</v>
+      </c>
+      <c r="B91">
+        <v>4</v>
+      </c>
+      <c r="C91">
+        <v>0.2</v>
+      </c>
+      <c r="D91" t="s">
+        <v>111</v>
+      </c>
+      <c r="E91" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="21">
-        <v>18</v>
-      </c>
-      <c r="B91">
-        <v>0</v>
-      </c>
-      <c r="C91">
-        <v>0.25</v>
-      </c>
-      <c r="D91" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="21">
         <v>18</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C92">
         <v>0.25</v>
       </c>
       <c r="D92" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="E92" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="21">
         <v>18</v>
       </c>
       <c r="B93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C93">
         <v>0.25</v>
       </c>
       <c r="D93" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="E93" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="21">
         <v>18</v>
       </c>
       <c r="B94">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C94">
         <v>0.25</v>
       </c>
       <c r="D94" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="E94" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="21">
         <v>18</v>
       </c>
       <c r="B95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C95">
         <v>0.25</v>
       </c>
       <c r="D95" t="s">
+        <v>112</v>
+      </c>
+      <c r="E95" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="21">
+        <v>18</v>
+      </c>
+      <c r="B96">
+        <v>4</v>
+      </c>
+      <c r="C96">
+        <v>0.25</v>
+      </c>
+      <c r="D96" t="s">
+        <v>112</v>
+      </c>
+      <c r="E96" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="22">
-        <v>19</v>
-      </c>
-      <c r="B96">
-        <v>0</v>
-      </c>
-      <c r="C96">
-        <v>0.88</v>
-      </c>
-      <c r="D96" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="22">
         <v>19</v>
       </c>
       <c r="B97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C97">
         <v>0.88</v>
       </c>
       <c r="D97" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="E97" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="22">
         <v>19</v>
       </c>
       <c r="B98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C98">
         <v>0.88</v>
       </c>
       <c r="D98" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="E98" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="22">
         <v>19</v>
       </c>
       <c r="B99">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C99">
         <v>0.88</v>
       </c>
-      <c r="D99" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D99" t="s">
+        <v>101</v>
+      </c>
+      <c r="E99" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="22">
         <v>19</v>
       </c>
       <c r="B100">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C100">
         <v>0.88</v>
       </c>
       <c r="D100" t="s">
+        <v>101</v>
+      </c>
+      <c r="E100" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="22">
+        <v>19</v>
+      </c>
+      <c r="B101">
+        <v>4</v>
+      </c>
+      <c r="C101">
+        <v>0.88</v>
+      </c>
+      <c r="D101" t="s">
+        <v>101</v>
+      </c>
+      <c r="E101" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D38" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D56" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D58" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D64" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D65" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D84" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D87" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D99" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D6" r:id="rId10" xr:uid="{FC5606A3-8740-497F-8803-BA54045ADE5D}"/>
-    <hyperlink ref="D11" r:id="rId11" xr:uid="{70FF1589-2B5F-427D-A47C-C183F02F81F9}"/>
-    <hyperlink ref="D12" r:id="rId12" xr:uid="{52F3720C-CC87-4B90-A31E-1696867E898C}"/>
-    <hyperlink ref="D13" r:id="rId13" xr:uid="{35D80060-F3E4-4D13-B568-5DFB4333DA7A}"/>
-    <hyperlink ref="D14" r:id="rId14" xr:uid="{0027613A-8A81-4481-883A-7F33A2EC06F5}"/>
-    <hyperlink ref="D15" r:id="rId15" xr:uid="{21B879B6-D217-4285-BA17-8B7D23C8C353}"/>
-    <hyperlink ref="D7" r:id="rId16" xr:uid="{3DEB9249-5488-473D-B912-5EE28D6183C9}"/>
-    <hyperlink ref="D8" r:id="rId17" xr:uid="{32991EE5-A126-41DF-8B9E-424E4002858D}"/>
-    <hyperlink ref="D9" r:id="rId18" xr:uid="{CD258F5E-54C0-461B-9F84-4FB1D287C54C}"/>
-    <hyperlink ref="D10" r:id="rId19" xr:uid="{963B8F45-B326-47EF-A0D2-942FE89A9C95}"/>
-    <hyperlink ref="D2" r:id="rId20" xr:uid="{0D6D5DF4-259A-4818-973B-FD7D7E0AC4A9}"/>
-    <hyperlink ref="D4" r:id="rId21" xr:uid="{085D0DBC-56B1-4B94-B0C1-34C1CD21C704}"/>
-    <hyperlink ref="D51" r:id="rId22" xr:uid="{3CAF7E62-1B02-4C8A-96DB-76B851A02BB8}"/>
-    <hyperlink ref="D52" r:id="rId23" xr:uid="{00447AF5-0568-4638-A15C-19D01D18ABC4}"/>
-    <hyperlink ref="D53" r:id="rId24" xr:uid="{72E88B7B-4CCD-4603-9DD7-ADC76D4831B6}"/>
-    <hyperlink ref="D54" r:id="rId25" xr:uid="{26023833-0476-4DA3-BD3A-898EDB41D1EC}"/>
-    <hyperlink ref="D55" r:id="rId26" xr:uid="{90A166D6-A445-455B-866D-EE99CDA5BDE8}"/>
-    <hyperlink ref="D46" r:id="rId27" xr:uid="{D8E511FF-DC35-47E0-863D-EBF7A6FF4802}"/>
-    <hyperlink ref="D47" r:id="rId28" xr:uid="{DAACB6E2-9A25-462C-85A1-5AAD01B90A5A}"/>
-    <hyperlink ref="D50" r:id="rId29" xr:uid="{38C6F7F3-40DE-4A43-BDDE-E296D4015F89}"/>
+    <hyperlink ref="E39" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E41" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E57" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E59" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E65" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E66" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E85" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E88" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E100" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E7" r:id="rId10" xr:uid="{FC5606A3-8740-497F-8803-BA54045ADE5D}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{70FF1589-2B5F-427D-A47C-C183F02F81F9}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{52F3720C-CC87-4B90-A31E-1696867E898C}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{35D80060-F3E4-4D13-B568-5DFB4333DA7A}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{0027613A-8A81-4481-883A-7F33A2EC06F5}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{21B879B6-D217-4285-BA17-8B7D23C8C353}"/>
+    <hyperlink ref="E8" r:id="rId16" xr:uid="{3DEB9249-5488-473D-B912-5EE28D6183C9}"/>
+    <hyperlink ref="E9" r:id="rId17" xr:uid="{32991EE5-A126-41DF-8B9E-424E4002858D}"/>
+    <hyperlink ref="E10" r:id="rId18" xr:uid="{CD258F5E-54C0-461B-9F84-4FB1D287C54C}"/>
+    <hyperlink ref="E11" r:id="rId19" xr:uid="{963B8F45-B326-47EF-A0D2-942FE89A9C95}"/>
+    <hyperlink ref="E3" r:id="rId20" xr:uid="{0D6D5DF4-259A-4818-973B-FD7D7E0AC4A9}"/>
+    <hyperlink ref="E5" r:id="rId21" xr:uid="{085D0DBC-56B1-4B94-B0C1-34C1CD21C704}"/>
+    <hyperlink ref="E52" r:id="rId22" xr:uid="{3CAF7E62-1B02-4C8A-96DB-76B851A02BB8}"/>
+    <hyperlink ref="E53" r:id="rId23" xr:uid="{00447AF5-0568-4638-A15C-19D01D18ABC4}"/>
+    <hyperlink ref="E54" r:id="rId24" xr:uid="{72E88B7B-4CCD-4603-9DD7-ADC76D4831B6}"/>
+    <hyperlink ref="E55" r:id="rId25" xr:uid="{26023833-0476-4DA3-BD3A-898EDB41D1EC}"/>
+    <hyperlink ref="E56" r:id="rId26" xr:uid="{90A166D6-A445-455B-866D-EE99CDA5BDE8}"/>
+    <hyperlink ref="E47" r:id="rId27" xr:uid="{D8E511FF-DC35-47E0-863D-EBF7A6FF4802}"/>
+    <hyperlink ref="E48" r:id="rId28" xr:uid="{DAACB6E2-9A25-462C-85A1-5AAD01B90A5A}"/>
+    <hyperlink ref="E51" r:id="rId29" xr:uid="{38C6F7F3-40DE-4A43-BDDE-E296D4015F89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added gallery category to table
</commit_message>
<xml_diff>
--- a/dataset/data-infos.xlsx
+++ b/dataset/data-infos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c4b1d2011ae4f894/Documents/GitHub/order_experiment/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:40009_{9D7C50B8-D3FB-4B8D-8E37-DD15650E8EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B0E5920-2EAC-40E4-A9BD-EE404DD7C565}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:40009_{9D7C50B8-D3FB-4B8D-8E37-DD15650E8EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9F61A80-656E-438B-AFFA-A7134EF98B27}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2925" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="119">
   <si>
     <t>https://opensea.io/assets/ethereum/0xcb1021080b61dac7032618de925a62176cbc8372/2547</t>
   </si>
@@ -374,6 +374,9 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -1373,15 +1376,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1395,10 +1398,13 @@
         <v>116</v>
       </c>
       <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1411,11 +1417,14 @@
       <c r="D2" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1428,11 +1437,14 @@
       <c r="D3" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1445,11 +1457,14 @@
       <c r="D4" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -1462,11 +1477,14 @@
       <c r="D5" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -1479,11 +1497,14 @@
       <c r="D6" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -1496,11 +1517,14 @@
       <c r="D7" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -1513,11 +1537,14 @@
       <c r="D8" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -1530,11 +1557,14 @@
       <c r="D9" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -1547,11 +1577,14 @@
       <c r="D10" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -1564,11 +1597,14 @@
       <c r="D11" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>2</v>
       </c>
@@ -1581,11 +1617,14 @@
       <c r="D12" t="s">
         <v>102</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>2</v>
       </c>
@@ -1598,11 +1637,14 @@
       <c r="D13" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>2</v>
       </c>
@@ -1615,11 +1657,14 @@
       <c r="D14" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -1632,11 +1677,14 @@
       <c r="D15" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>2</v>
       </c>
@@ -1649,11 +1697,14 @@
       <c r="D16" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>3</v>
       </c>
@@ -1666,11 +1717,14 @@
       <c r="D17" t="s">
         <v>103</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>3</v>
       </c>
@@ -1683,11 +1737,14 @@
       <c r="D18" t="s">
         <v>103</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>3</v>
       </c>
@@ -1700,11 +1757,14 @@
       <c r="D19" t="s">
         <v>103</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>3</v>
       </c>
@@ -1717,11 +1777,14 @@
       <c r="D20" t="s">
         <v>103</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>3</v>
       </c>
@@ -1734,11 +1797,14 @@
       <c r="D21" t="s">
         <v>103</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>4</v>
       </c>
@@ -1751,11 +1817,14 @@
       <c r="D22" t="s">
         <v>104</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>4</v>
       </c>
@@ -1768,11 +1837,14 @@
       <c r="D23" t="s">
         <v>104</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>4</v>
       </c>
@@ -1785,11 +1857,14 @@
       <c r="D24" t="s">
         <v>104</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>4</v>
       </c>
@@ -1802,11 +1877,14 @@
       <c r="D25" t="s">
         <v>104</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>4</v>
       </c>
@@ -1819,11 +1897,14 @@
       <c r="D26" t="s">
         <v>104</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>5</v>
       </c>
@@ -1836,11 +1917,14 @@
       <c r="D27" t="s">
         <v>105</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>5</v>
       </c>
@@ -1853,11 +1937,14 @@
       <c r="D28" t="s">
         <v>105</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>5</v>
       </c>
@@ -1870,11 +1957,14 @@
       <c r="D29" t="s">
         <v>105</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>5</v>
       </c>
@@ -1887,11 +1977,14 @@
       <c r="D30" t="s">
         <v>105</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>5</v>
       </c>
@@ -1904,11 +1997,14 @@
       <c r="D31" t="s">
         <v>105</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>6</v>
       </c>
@@ -1921,11 +2017,14 @@
       <c r="D32" t="s">
         <v>102</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>6</v>
       </c>
@@ -1938,11 +2037,14 @@
       <c r="D33" t="s">
         <v>102</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>6</v>
       </c>
@@ -1955,11 +2057,14 @@
       <c r="D34" t="s">
         <v>102</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>6</v>
       </c>
@@ -1972,11 +2077,14 @@
       <c r="D35" t="s">
         <v>102</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>6</v>
       </c>
@@ -1989,11 +2097,14 @@
       <c r="D36" t="s">
         <v>102</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>7</v>
       </c>
@@ -2006,11 +2117,14 @@
       <c r="D37" t="s">
         <v>101</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>7</v>
       </c>
@@ -2023,11 +2137,14 @@
       <c r="D38" t="s">
         <v>101</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>7</v>
       </c>
@@ -2040,11 +2157,14 @@
       <c r="D39" t="s">
         <v>101</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>7</v>
       </c>
@@ -2057,11 +2177,14 @@
       <c r="D40" t="s">
         <v>101</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>7</v>
       </c>
@@ -2074,11 +2197,14 @@
       <c r="D41" t="s">
         <v>101</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="9">
         <v>8</v>
       </c>
@@ -2091,11 +2217,14 @@
       <c r="D42" t="s">
         <v>106</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -2108,11 +2237,14 @@
       <c r="D43" t="s">
         <v>106</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
         <v>8</v>
       </c>
@@ -2125,11 +2257,14 @@
       <c r="D44" t="s">
         <v>106</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="9">
         <v>8</v>
       </c>
@@ -2142,11 +2277,14 @@
       <c r="D45" t="s">
         <v>106</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="9">
         <v>8</v>
       </c>
@@ -2159,11 +2297,14 @@
       <c r="D46" t="s">
         <v>106</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="10">
         <v>9</v>
       </c>
@@ -2176,11 +2317,14 @@
       <c r="D47" t="s">
         <v>106</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="10">
         <v>9</v>
       </c>
@@ -2193,11 +2337,14 @@
       <c r="D48" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="10">
         <v>9</v>
       </c>
@@ -2210,11 +2357,14 @@
       <c r="D49" t="s">
         <v>106</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="10">
         <v>9</v>
       </c>
@@ -2227,11 +2377,14 @@
       <c r="D50" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="10">
         <v>9</v>
       </c>
@@ -2244,11 +2397,14 @@
       <c r="D51" t="s">
         <v>106</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="13">
         <v>10</v>
       </c>
@@ -2261,11 +2417,14 @@
       <c r="D52" t="s">
         <v>107</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>10</v>
       </c>
@@ -2278,11 +2437,14 @@
       <c r="D53" t="s">
         <v>107</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="13">
         <v>10</v>
       </c>
@@ -2295,11 +2457,14 @@
       <c r="D54" t="s">
         <v>107</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="13">
         <v>10</v>
       </c>
@@ -2312,11 +2477,14 @@
       <c r="D55" t="s">
         <v>107</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="13">
         <v>10</v>
       </c>
@@ -2329,11 +2497,14 @@
       <c r="D56" t="s">
         <v>107</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
         <v>11</v>
       </c>
@@ -2346,11 +2517,14 @@
       <c r="D57" t="s">
         <v>108</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
         <v>11</v>
       </c>
@@ -2363,11 +2537,14 @@
       <c r="D58" t="s">
         <v>108</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="14">
         <v>11</v>
       </c>
@@ -2380,11 +2557,14 @@
       <c r="D59" t="s">
         <v>108</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="14">
         <v>11</v>
       </c>
@@ -2397,11 +2577,14 @@
       <c r="D60" t="s">
         <v>108</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="14">
         <v>11</v>
       </c>
@@ -2414,11 +2597,14 @@
       <c r="D61" t="s">
         <v>108</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <v>12</v>
       </c>
@@ -2431,11 +2617,14 @@
       <c r="D62" t="s">
         <v>104</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="15">
         <v>12</v>
       </c>
@@ -2448,11 +2637,14 @@
       <c r="D63" t="s">
         <v>104</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="15">
         <v>12</v>
       </c>
@@ -2465,11 +2657,14 @@
       <c r="D64" t="s">
         <v>104</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <v>12</v>
       </c>
@@ -2482,11 +2677,14 @@
       <c r="D65" t="s">
         <v>104</v>
       </c>
-      <c r="E65" s="11" t="s">
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="15">
         <v>12</v>
       </c>
@@ -2499,11 +2697,14 @@
       <c r="D66" t="s">
         <v>104</v>
       </c>
-      <c r="E66" s="11" t="s">
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="16">
         <v>13</v>
       </c>
@@ -2516,11 +2717,14 @@
       <c r="D67" t="s">
         <v>109</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="16">
         <v>13</v>
       </c>
@@ -2533,11 +2737,14 @@
       <c r="D68" t="s">
         <v>109</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="16">
         <v>13</v>
       </c>
@@ -2550,11 +2757,14 @@
       <c r="D69" t="s">
         <v>109</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="16">
         <v>13</v>
       </c>
@@ -2567,11 +2777,14 @@
       <c r="D70" t="s">
         <v>109</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="16">
         <v>13</v>
       </c>
@@ -2584,11 +2797,14 @@
       <c r="D71" t="s">
         <v>109</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="17">
         <v>14</v>
       </c>
@@ -2601,11 +2817,14 @@
       <c r="D72" t="s">
         <v>103</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="17">
         <v>14</v>
       </c>
@@ -2618,11 +2837,14 @@
       <c r="D73" t="s">
         <v>103</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="17">
         <v>14</v>
       </c>
@@ -2635,11 +2857,14 @@
       <c r="D74" t="s">
         <v>103</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="17">
         <v>14</v>
       </c>
@@ -2652,11 +2877,14 @@
       <c r="D75" t="s">
         <v>103</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="17">
         <v>14</v>
       </c>
@@ -2669,11 +2897,14 @@
       <c r="D76" t="s">
         <v>103</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="18">
         <v>15</v>
       </c>
@@ -2686,11 +2917,14 @@
       <c r="D77" t="s">
         <v>110</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="F77" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="18">
         <v>15</v>
       </c>
@@ -2703,11 +2937,14 @@
       <c r="D78" t="s">
         <v>110</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="F78" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="18">
         <v>15</v>
       </c>
@@ -2720,11 +2957,14 @@
       <c r="D79" t="s">
         <v>110</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="F79" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="18">
         <v>15</v>
       </c>
@@ -2737,11 +2977,14 @@
       <c r="D80" t="s">
         <v>110</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="18">
         <v>15</v>
       </c>
@@ -2754,11 +2997,14 @@
       <c r="D81" t="s">
         <v>110</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="F81" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="19">
         <v>16</v>
       </c>
@@ -2771,11 +3017,14 @@
       <c r="D82" t="s">
         <v>111</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82">
+        <v>2</v>
+      </c>
+      <c r="F82" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="19">
         <v>16</v>
       </c>
@@ -2788,11 +3037,14 @@
       <c r="D83" t="s">
         <v>111</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="F83" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="19">
         <v>16</v>
       </c>
@@ -2805,11 +3057,14 @@
       <c r="D84" t="s">
         <v>111</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="19">
         <v>16</v>
       </c>
@@ -2822,11 +3077,14 @@
       <c r="D85" t="s">
         <v>111</v>
       </c>
-      <c r="E85" s="11" t="s">
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="F85" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="19">
         <v>16</v>
       </c>
@@ -2839,11 +3097,14 @@
       <c r="D86" t="s">
         <v>111</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="F86" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="20">
         <v>17</v>
       </c>
@@ -2856,11 +3117,14 @@
       <c r="D87" t="s">
         <v>111</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87">
+        <v>2</v>
+      </c>
+      <c r="F87" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="20">
         <v>17</v>
       </c>
@@ -2873,11 +3137,14 @@
       <c r="D88" t="s">
         <v>111</v>
       </c>
-      <c r="E88" s="11" t="s">
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="F88" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="20">
         <v>17</v>
       </c>
@@ -2890,11 +3157,14 @@
       <c r="D89" t="s">
         <v>111</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89">
+        <v>2</v>
+      </c>
+      <c r="F89" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="20">
         <v>17</v>
       </c>
@@ -2907,11 +3177,14 @@
       <c r="D90" t="s">
         <v>111</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90">
+        <v>2</v>
+      </c>
+      <c r="F90" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="20">
         <v>17</v>
       </c>
@@ -2924,11 +3197,14 @@
       <c r="D91" t="s">
         <v>111</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91">
+        <v>2</v>
+      </c>
+      <c r="F91" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="21">
         <v>18</v>
       </c>
@@ -2941,11 +3217,14 @@
       <c r="D92" t="s">
         <v>112</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="F92" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="21">
         <v>18</v>
       </c>
@@ -2958,11 +3237,14 @@
       <c r="D93" t="s">
         <v>112</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93">
+        <v>2</v>
+      </c>
+      <c r="F93" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="21">
         <v>18</v>
       </c>
@@ -2975,11 +3257,14 @@
       <c r="D94" t="s">
         <v>112</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="21">
         <v>18</v>
       </c>
@@ -2992,11 +3277,14 @@
       <c r="D95" t="s">
         <v>112</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95">
+        <v>2</v>
+      </c>
+      <c r="F95" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="21">
         <v>18</v>
       </c>
@@ -3009,11 +3297,14 @@
       <c r="D96" t="s">
         <v>112</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96">
+        <v>2</v>
+      </c>
+      <c r="F96" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="22">
         <v>19</v>
       </c>
@@ -3026,11 +3317,14 @@
       <c r="D97" t="s">
         <v>101</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97">
+        <v>2</v>
+      </c>
+      <c r="F97" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="22">
         <v>19</v>
       </c>
@@ -3043,11 +3337,14 @@
       <c r="D98" t="s">
         <v>101</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98">
+        <v>2</v>
+      </c>
+      <c r="F98" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="22">
         <v>19</v>
       </c>
@@ -3060,11 +3357,14 @@
       <c r="D99" t="s">
         <v>101</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99">
+        <v>2</v>
+      </c>
+      <c r="F99" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="22">
         <v>19</v>
       </c>
@@ -3077,11 +3377,14 @@
       <c r="D100" t="s">
         <v>101</v>
       </c>
-      <c r="E100" s="11" t="s">
+      <c r="E100">
+        <v>2</v>
+      </c>
+      <c r="F100" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="22">
         <v>19</v>
       </c>
@@ -3094,41 +3397,44 @@
       <c r="D101" t="s">
         <v>101</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101">
+        <v>2</v>
+      </c>
+      <c r="F101" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E39" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E41" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E57" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E59" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E65" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E66" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E85" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E88" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E100" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E7" r:id="rId10" xr:uid="{FC5606A3-8740-497F-8803-BA54045ADE5D}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{70FF1589-2B5F-427D-A47C-C183F02F81F9}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{52F3720C-CC87-4B90-A31E-1696867E898C}"/>
-    <hyperlink ref="E14" r:id="rId13" xr:uid="{35D80060-F3E4-4D13-B568-5DFB4333DA7A}"/>
-    <hyperlink ref="E15" r:id="rId14" xr:uid="{0027613A-8A81-4481-883A-7F33A2EC06F5}"/>
-    <hyperlink ref="E16" r:id="rId15" xr:uid="{21B879B6-D217-4285-BA17-8B7D23C8C353}"/>
-    <hyperlink ref="E8" r:id="rId16" xr:uid="{3DEB9249-5488-473D-B912-5EE28D6183C9}"/>
-    <hyperlink ref="E9" r:id="rId17" xr:uid="{32991EE5-A126-41DF-8B9E-424E4002858D}"/>
-    <hyperlink ref="E10" r:id="rId18" xr:uid="{CD258F5E-54C0-461B-9F84-4FB1D287C54C}"/>
-    <hyperlink ref="E11" r:id="rId19" xr:uid="{963B8F45-B326-47EF-A0D2-942FE89A9C95}"/>
-    <hyperlink ref="E3" r:id="rId20" xr:uid="{0D6D5DF4-259A-4818-973B-FD7D7E0AC4A9}"/>
-    <hyperlink ref="E5" r:id="rId21" xr:uid="{085D0DBC-56B1-4B94-B0C1-34C1CD21C704}"/>
-    <hyperlink ref="E52" r:id="rId22" xr:uid="{3CAF7E62-1B02-4C8A-96DB-76B851A02BB8}"/>
-    <hyperlink ref="E53" r:id="rId23" xr:uid="{00447AF5-0568-4638-A15C-19D01D18ABC4}"/>
-    <hyperlink ref="E54" r:id="rId24" xr:uid="{72E88B7B-4CCD-4603-9DD7-ADC76D4831B6}"/>
-    <hyperlink ref="E55" r:id="rId25" xr:uid="{26023833-0476-4DA3-BD3A-898EDB41D1EC}"/>
-    <hyperlink ref="E56" r:id="rId26" xr:uid="{90A166D6-A445-455B-866D-EE99CDA5BDE8}"/>
-    <hyperlink ref="E47" r:id="rId27" xr:uid="{D8E511FF-DC35-47E0-863D-EBF7A6FF4802}"/>
-    <hyperlink ref="E48" r:id="rId28" xr:uid="{DAACB6E2-9A25-462C-85A1-5AAD01B90A5A}"/>
-    <hyperlink ref="E51" r:id="rId29" xr:uid="{38C6F7F3-40DE-4A43-BDDE-E296D4015F89}"/>
+    <hyperlink ref="F39" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F41" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F57" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F59" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F65" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F66" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F85" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F88" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F100" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F7" r:id="rId10" xr:uid="{FC5606A3-8740-497F-8803-BA54045ADE5D}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{70FF1589-2B5F-427D-A47C-C183F02F81F9}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{52F3720C-CC87-4B90-A31E-1696867E898C}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{35D80060-F3E4-4D13-B568-5DFB4333DA7A}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{0027613A-8A81-4481-883A-7F33A2EC06F5}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{21B879B6-D217-4285-BA17-8B7D23C8C353}"/>
+    <hyperlink ref="F8" r:id="rId16" xr:uid="{3DEB9249-5488-473D-B912-5EE28D6183C9}"/>
+    <hyperlink ref="F9" r:id="rId17" xr:uid="{32991EE5-A126-41DF-8B9E-424E4002858D}"/>
+    <hyperlink ref="F10" r:id="rId18" xr:uid="{CD258F5E-54C0-461B-9F84-4FB1D287C54C}"/>
+    <hyperlink ref="F11" r:id="rId19" xr:uid="{963B8F45-B326-47EF-A0D2-942FE89A9C95}"/>
+    <hyperlink ref="F3" r:id="rId20" xr:uid="{0D6D5DF4-259A-4818-973B-FD7D7E0AC4A9}"/>
+    <hyperlink ref="F5" r:id="rId21" xr:uid="{085D0DBC-56B1-4B94-B0C1-34C1CD21C704}"/>
+    <hyperlink ref="F52" r:id="rId22" xr:uid="{3CAF7E62-1B02-4C8A-96DB-76B851A02BB8}"/>
+    <hyperlink ref="F53" r:id="rId23" xr:uid="{00447AF5-0568-4638-A15C-19D01D18ABC4}"/>
+    <hyperlink ref="F54" r:id="rId24" xr:uid="{72E88B7B-4CCD-4603-9DD7-ADC76D4831B6}"/>
+    <hyperlink ref="F55" r:id="rId25" xr:uid="{26023833-0476-4DA3-BD3A-898EDB41D1EC}"/>
+    <hyperlink ref="F56" r:id="rId26" xr:uid="{90A166D6-A445-455B-866D-EE99CDA5BDE8}"/>
+    <hyperlink ref="F47" r:id="rId27" xr:uid="{D8E511FF-DC35-47E0-863D-EBF7A6FF4802}"/>
+    <hyperlink ref="F48" r:id="rId28" xr:uid="{DAACB6E2-9A25-462C-85A1-5AAD01B90A5A}"/>
+    <hyperlink ref="F51" r:id="rId29" xr:uid="{38C6F7F3-40DE-4A43-BDDE-E296D4015F89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed decimal separator to dot
</commit_message>
<xml_diff>
--- a/dataset/data-infos.xlsx
+++ b/dataset/data-infos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c4b1d2011ae4f894/Documents/GitHub/order_experiment/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:40009_{9D7C50B8-D3FB-4B8D-8E37-DD15650E8EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9F61A80-656E-438B-AFFA-A7134EF98B27}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="13_ncr:40009_{9D7C50B8-D3FB-4B8D-8E37-DD15650E8EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F078A407-1AFD-41BF-954B-60A0C5C45601}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2925" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="167">
   <si>
     <t>https://opensea.io/assets/ethereum/0xcb1021080b61dac7032618de925a62176cbc8372/2547</t>
   </si>
@@ -377,12 +377,159 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.17</t>
+  </si>
+  <si>
+    <t>0.1499</t>
+  </si>
+  <si>
+    <t>0.129</t>
+  </si>
+  <si>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>1.99</t>
+  </si>
+  <si>
+    <t>1.111</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>0.78</t>
+  </si>
+  <si>
+    <t>28.75</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>0.4207</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>0.69</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>0.349</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>1.65</t>
+  </si>
+  <si>
+    <t>1.25</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>85.69</t>
+  </si>
+  <si>
+    <t>40.666</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>1.38</t>
+  </si>
+  <si>
+    <t>0.39</t>
+  </si>
+  <si>
+    <t>0.32</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.37</t>
+  </si>
+  <si>
+    <t>0.295</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>0.419</t>
+  </si>
+  <si>
+    <t>0.339</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>0.028</t>
+  </si>
+  <si>
+    <t>0.026</t>
+  </si>
+  <si>
+    <t>29.37</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.21</t>
+  </si>
+  <si>
+    <t>0.88</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -951,7 +1098,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -995,8 +1142,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1009,7 +1157,6 @@
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
@@ -1020,8 +1167,10 @@
     <xf numFmtId="0" fontId="17" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1049,6 +1198,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="43" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1378,11 +1528,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1411,8 +1564,8 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>0.2</v>
+      <c r="C2" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="D2" t="s">
         <v>100</v>
@@ -1431,8 +1584,8 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>0.17</v>
+      <c r="C3" s="22" t="s">
+        <v>120</v>
       </c>
       <c r="D3" t="s">
         <v>100</v>
@@ -1451,8 +1604,8 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>0.14990000000000001</v>
+      <c r="C4" s="22" t="s">
+        <v>121</v>
       </c>
       <c r="D4" t="s">
         <v>100</v>
@@ -1471,8 +1624,8 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>0.129</v>
+      <c r="C5" s="22" t="s">
+        <v>122</v>
       </c>
       <c r="D5" t="s">
         <v>100</v>
@@ -1491,8 +1644,8 @@
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>0.12</v>
+      <c r="C6" s="22" t="s">
+        <v>123</v>
       </c>
       <c r="D6" t="s">
         <v>100</v>
@@ -1511,8 +1664,8 @@
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>3.1</v>
+      <c r="C7" s="22" t="s">
+        <v>124</v>
       </c>
       <c r="D7" t="s">
         <v>101</v>
@@ -1531,8 +1684,8 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>1.99</v>
+      <c r="C8" s="22" t="s">
+        <v>125</v>
       </c>
       <c r="D8" t="s">
         <v>101</v>
@@ -1551,8 +1704,8 @@
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9">
-        <v>1.111</v>
+      <c r="C9" s="22" t="s">
+        <v>126</v>
       </c>
       <c r="D9" t="s">
         <v>101</v>
@@ -1571,8 +1724,8 @@
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10">
-        <v>0.9</v>
+      <c r="C10" s="22" t="s">
+        <v>127</v>
       </c>
       <c r="D10" t="s">
         <v>101</v>
@@ -1591,8 +1744,8 @@
       <c r="B11">
         <v>4</v>
       </c>
-      <c r="C11">
-        <v>0.75</v>
+      <c r="C11" s="22" t="s">
+        <v>128</v>
       </c>
       <c r="D11" t="s">
         <v>101</v>
@@ -1611,7 +1764,7 @@
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="22">
         <v>1</v>
       </c>
       <c r="D12" t="s">
@@ -1631,8 +1784,8 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13">
-        <v>0.5</v>
+      <c r="C13" s="22" t="s">
+        <v>129</v>
       </c>
       <c r="D13" t="s">
         <v>102</v>
@@ -1651,8 +1804,8 @@
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14">
-        <v>0.38</v>
+      <c r="C14" s="22" t="s">
+        <v>130</v>
       </c>
       <c r="D14" t="s">
         <v>102</v>
@@ -1671,8 +1824,8 @@
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="C15">
-        <v>0.2</v>
+      <c r="C15" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="D15" t="s">
         <v>102</v>
@@ -1691,8 +1844,8 @@
       <c r="B16">
         <v>4</v>
       </c>
-      <c r="C16">
-        <v>0.78</v>
+      <c r="C16" s="22" t="s">
+        <v>131</v>
       </c>
       <c r="D16" t="s">
         <v>102</v>
@@ -1711,7 +1864,7 @@
       <c r="B17">
         <v>0</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="22">
         <v>75</v>
       </c>
       <c r="D17" t="s">
@@ -1731,7 +1884,7 @@
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="22">
         <v>55</v>
       </c>
       <c r="D18" t="s">
@@ -1751,7 +1904,7 @@
       <c r="B19">
         <v>2</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="22">
         <v>45</v>
       </c>
       <c r="D19" t="s">
@@ -1771,8 +1924,8 @@
       <c r="B20">
         <v>3</v>
       </c>
-      <c r="C20">
-        <v>28.75</v>
+      <c r="C20" s="22" t="s">
+        <v>132</v>
       </c>
       <c r="D20" t="s">
         <v>103</v>
@@ -1791,7 +1944,7 @@
       <c r="B21">
         <v>4</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="22">
         <v>15</v>
       </c>
       <c r="D21" t="s">
@@ -1811,8 +1964,8 @@
       <c r="B22">
         <v>0</v>
       </c>
-      <c r="C22">
-        <v>1.2</v>
+      <c r="C22" s="22" t="s">
+        <v>133</v>
       </c>
       <c r="D22" t="s">
         <v>104</v>
@@ -1831,7 +1984,7 @@
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="22">
         <v>1</v>
       </c>
       <c r="D23" t="s">
@@ -1851,8 +2004,8 @@
       <c r="B24">
         <v>2</v>
       </c>
-      <c r="C24">
-        <v>0.75</v>
+      <c r="C24" s="22" t="s">
+        <v>128</v>
       </c>
       <c r="D24" t="s">
         <v>104</v>
@@ -1871,8 +2024,8 @@
       <c r="B25">
         <v>3</v>
       </c>
-      <c r="C25">
-        <v>0.5</v>
+      <c r="C25" s="22" t="s">
+        <v>129</v>
       </c>
       <c r="D25" t="s">
         <v>104</v>
@@ -1891,8 +2044,8 @@
       <c r="B26">
         <v>4</v>
       </c>
-      <c r="C26">
-        <v>0.42070000000000002</v>
+      <c r="C26" s="22" t="s">
+        <v>134</v>
       </c>
       <c r="D26" t="s">
         <v>104</v>
@@ -1911,7 +2064,7 @@
       <c r="B27">
         <v>0</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="22">
         <v>2</v>
       </c>
       <c r="D27" t="s">
@@ -1931,8 +2084,8 @@
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28">
-        <v>1.2</v>
+      <c r="C28" s="22" t="s">
+        <v>133</v>
       </c>
       <c r="D28" t="s">
         <v>105</v>
@@ -1951,8 +2104,8 @@
       <c r="B29">
         <v>2</v>
       </c>
-      <c r="C29">
-        <v>0.99</v>
+      <c r="C29" s="22" t="s">
+        <v>135</v>
       </c>
       <c r="D29" t="s">
         <v>105</v>
@@ -1971,8 +2124,8 @@
       <c r="B30">
         <v>3</v>
       </c>
-      <c r="C30">
-        <v>0.69</v>
+      <c r="C30" s="22" t="s">
+        <v>136</v>
       </c>
       <c r="D30" t="s">
         <v>105</v>
@@ -1991,8 +2144,8 @@
       <c r="B31">
         <v>4</v>
       </c>
-      <c r="C31">
-        <v>0.25</v>
+      <c r="C31" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D31" t="s">
         <v>105</v>
@@ -2011,7 +2164,7 @@
       <c r="B32">
         <v>0</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="22">
         <v>1</v>
       </c>
       <c r="D32" t="s">
@@ -2031,8 +2184,8 @@
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33">
-        <v>0.8</v>
+      <c r="C33" s="22" t="s">
+        <v>138</v>
       </c>
       <c r="D33" t="s">
         <v>102</v>
@@ -2051,8 +2204,8 @@
       <c r="B34">
         <v>2</v>
       </c>
-      <c r="C34">
-        <v>0.68</v>
+      <c r="C34" s="22" t="s">
+        <v>139</v>
       </c>
       <c r="D34" t="s">
         <v>102</v>
@@ -2071,8 +2224,8 @@
       <c r="B35">
         <v>3</v>
       </c>
-      <c r="C35">
-        <v>0.5</v>
+      <c r="C35" s="22" t="s">
+        <v>129</v>
       </c>
       <c r="D35" t="s">
         <v>102</v>
@@ -2091,8 +2244,8 @@
       <c r="B36">
         <v>4</v>
       </c>
-      <c r="C36">
-        <v>0.34899999999999998</v>
+      <c r="C36" s="22" t="s">
+        <v>140</v>
       </c>
       <c r="D36" t="s">
         <v>102</v>
@@ -2111,8 +2264,8 @@
       <c r="B37">
         <v>0</v>
       </c>
-      <c r="C37">
-        <v>2.5</v>
+      <c r="C37" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="D37" t="s">
         <v>101</v>
@@ -2131,8 +2284,8 @@
       <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38">
-        <v>2.2000000000000002</v>
+      <c r="C38" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="D38" t="s">
         <v>101</v>
@@ -2151,8 +2304,8 @@
       <c r="B39">
         <v>2</v>
       </c>
-      <c r="C39">
-        <v>1.65</v>
+      <c r="C39" s="22" t="s">
+        <v>143</v>
       </c>
       <c r="D39" t="s">
         <v>101</v>
@@ -2171,8 +2324,8 @@
       <c r="B40">
         <v>3</v>
       </c>
-      <c r="C40">
-        <v>1.25</v>
+      <c r="C40" s="22" t="s">
+        <v>144</v>
       </c>
       <c r="D40" t="s">
         <v>101</v>
@@ -2191,8 +2344,8 @@
       <c r="B41">
         <v>4</v>
       </c>
-      <c r="C41">
-        <v>0.98</v>
+      <c r="C41" s="22" t="s">
+        <v>145</v>
       </c>
       <c r="D41" t="s">
         <v>101</v>
@@ -2211,7 +2364,7 @@
       <c r="B42">
         <v>0</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="22">
         <v>130</v>
       </c>
       <c r="D42" t="s">
@@ -2231,7 +2384,7 @@
       <c r="B43">
         <v>1</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="22">
         <v>100</v>
       </c>
       <c r="D43" t="s">
@@ -2251,7 +2404,7 @@
       <c r="B44">
         <v>2</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="22">
         <v>69</v>
       </c>
       <c r="D44" t="s">
@@ -2271,7 +2424,7 @@
       <c r="B45">
         <v>3</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="22">
         <v>49</v>
       </c>
       <c r="D45" t="s">
@@ -2291,7 +2444,7 @@
       <c r="B46">
         <v>4</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="22">
         <v>30</v>
       </c>
       <c r="D46" t="s">
@@ -2311,7 +2464,7 @@
       <c r="B47">
         <v>0</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="22">
         <v>100</v>
       </c>
       <c r="D47" t="s">
@@ -2331,8 +2484,8 @@
       <c r="B48">
         <v>1</v>
       </c>
-      <c r="C48">
-        <v>85.69</v>
+      <c r="C48" s="22" t="s">
+        <v>146</v>
       </c>
       <c r="D48" t="s">
         <v>106</v>
@@ -2351,7 +2504,7 @@
       <c r="B49">
         <v>2</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="22">
         <v>55</v>
       </c>
       <c r="D49" t="s">
@@ -2371,8 +2524,8 @@
       <c r="B50">
         <v>3</v>
       </c>
-      <c r="C50">
-        <v>40.665999999999997</v>
+      <c r="C50" s="22" t="s">
+        <v>147</v>
       </c>
       <c r="D50" t="s">
         <v>106</v>
@@ -2391,8 +2544,8 @@
       <c r="B51">
         <v>4</v>
       </c>
-      <c r="C51">
-        <v>4.5</v>
+      <c r="C51" s="22" t="s">
+        <v>148</v>
       </c>
       <c r="D51" t="s">
         <v>106</v>
@@ -2405,14 +2558,14 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="13">
+      <c r="A52" s="12">
         <v>10</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
-      <c r="C52">
-        <v>1.38</v>
+      <c r="C52" s="22" t="s">
+        <v>149</v>
       </c>
       <c r="D52" t="s">
         <v>107</v>
@@ -2425,14 +2578,14 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="13">
+      <c r="A53" s="12">
         <v>10</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
-      <c r="C53">
-        <v>0.5</v>
+      <c r="C53" s="22" t="s">
+        <v>129</v>
       </c>
       <c r="D53" t="s">
         <v>107</v>
@@ -2445,14 +2598,14 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="13">
+      <c r="A54" s="12">
         <v>10</v>
       </c>
       <c r="B54">
         <v>2</v>
       </c>
-      <c r="C54">
-        <v>0.39</v>
+      <c r="C54" s="22" t="s">
+        <v>150</v>
       </c>
       <c r="D54" t="s">
         <v>107</v>
@@ -2465,14 +2618,14 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="13">
+      <c r="A55" s="12">
         <v>10</v>
       </c>
       <c r="B55">
         <v>3</v>
       </c>
-      <c r="C55" s="12">
-        <v>0.32</v>
+      <c r="C55" s="23" t="s">
+        <v>151</v>
       </c>
       <c r="D55" t="s">
         <v>107</v>
@@ -2485,14 +2638,14 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="13">
+      <c r="A56" s="12">
         <v>10</v>
       </c>
       <c r="B56">
         <v>4</v>
       </c>
-      <c r="C56">
-        <v>0.3</v>
+      <c r="C56" s="22" t="s">
+        <v>152</v>
       </c>
       <c r="D56" t="s">
         <v>107</v>
@@ -2505,14 +2658,14 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="14">
+      <c r="A57" s="13">
         <v>11</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
-      <c r="C57">
-        <v>0.37</v>
+      <c r="C57" s="22" t="s">
+        <v>153</v>
       </c>
       <c r="D57" t="s">
         <v>108</v>
@@ -2525,14 +2678,14 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="14">
+      <c r="A58" s="13">
         <v>11</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
-      <c r="C58">
-        <v>0.29499999999999998</v>
+      <c r="C58" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="D58" t="s">
         <v>108</v>
@@ -2545,14 +2698,14 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="14">
+      <c r="A59" s="13">
         <v>11</v>
       </c>
       <c r="B59">
         <v>2</v>
       </c>
-      <c r="C59">
-        <v>0.25</v>
+      <c r="C59" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D59" t="s">
         <v>108</v>
@@ -2565,14 +2718,14 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="14">
+      <c r="A60" s="13">
         <v>11</v>
       </c>
       <c r="B60">
         <v>3</v>
       </c>
-      <c r="C60">
-        <v>0.15</v>
+      <c r="C60" s="22" t="s">
+        <v>155</v>
       </c>
       <c r="D60" t="s">
         <v>108</v>
@@ -2585,14 +2738,14 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="14">
+      <c r="A61" s="13">
         <v>11</v>
       </c>
       <c r="B61">
         <v>4</v>
       </c>
-      <c r="C61">
-        <v>0.12</v>
+      <c r="C61" s="22" t="s">
+        <v>123</v>
       </c>
       <c r="D61" t="s">
         <v>108</v>
@@ -2605,14 +2758,14 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="15">
+      <c r="A62" s="14">
         <v>12</v>
       </c>
       <c r="B62">
         <v>0</v>
       </c>
-      <c r="C62">
-        <v>0.48</v>
+      <c r="C62" s="22" t="s">
+        <v>156</v>
       </c>
       <c r="D62" t="s">
         <v>104</v>
@@ -2625,14 +2778,14 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="15">
+      <c r="A63" s="14">
         <v>12</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
-      <c r="C63">
-        <v>0.41899999999999998</v>
+      <c r="C63" s="22" t="s">
+        <v>157</v>
       </c>
       <c r="D63" t="s">
         <v>104</v>
@@ -2645,14 +2798,14 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="15">
+      <c r="A64" s="14">
         <v>12</v>
       </c>
       <c r="B64">
         <v>2</v>
       </c>
-      <c r="C64">
-        <v>0.33900000000000002</v>
+      <c r="C64" s="22" t="s">
+        <v>158</v>
       </c>
       <c r="D64" t="s">
         <v>104</v>
@@ -2665,14 +2818,14 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="15">
+      <c r="A65" s="14">
         <v>12</v>
       </c>
       <c r="B65">
         <v>3</v>
       </c>
-      <c r="C65">
-        <v>0.25</v>
+      <c r="C65" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D65" t="s">
         <v>104</v>
@@ -2685,14 +2838,14 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="15">
+      <c r="A66" s="14">
         <v>12</v>
       </c>
       <c r="B66">
         <v>4</v>
       </c>
-      <c r="C66">
-        <v>0.2</v>
+      <c r="C66" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="D66" t="s">
         <v>104</v>
@@ -2705,14 +2858,14 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="16">
+      <c r="A67" s="15">
         <v>13</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
-      <c r="C67">
-        <v>0.05</v>
+      <c r="C67" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="D67" t="s">
         <v>109</v>
@@ -2720,19 +2873,19 @@
       <c r="E67">
         <v>1</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="11" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="16">
+      <c r="A68" s="15">
         <v>13</v>
       </c>
       <c r="B68">
         <v>1</v>
       </c>
-      <c r="C68">
-        <v>0.04</v>
+      <c r="C68" s="22" t="s">
+        <v>160</v>
       </c>
       <c r="D68" t="s">
         <v>109</v>
@@ -2745,14 +2898,14 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="16">
+      <c r="A69" s="15">
         <v>13</v>
       </c>
       <c r="B69">
         <v>2</v>
       </c>
-      <c r="C69">
-        <v>0.32</v>
+      <c r="C69" s="22" t="s">
+        <v>151</v>
       </c>
       <c r="D69" t="s">
         <v>109</v>
@@ -2765,14 +2918,14 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="16">
+      <c r="A70" s="15">
         <v>13</v>
       </c>
       <c r="B70">
         <v>3</v>
       </c>
-      <c r="C70">
-        <v>2.8000000000000001E-2</v>
+      <c r="C70" s="22" t="s">
+        <v>161</v>
       </c>
       <c r="D70" t="s">
         <v>109</v>
@@ -2785,14 +2938,14 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="16">
+      <c r="A71" s="15">
         <v>13</v>
       </c>
       <c r="B71">
         <v>4</v>
       </c>
-      <c r="C71">
-        <v>2.5999999999999999E-2</v>
+      <c r="C71" s="22" t="s">
+        <v>162</v>
       </c>
       <c r="D71" t="s">
         <v>109</v>
@@ -2805,13 +2958,13 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="17">
+      <c r="A72" s="16">
         <v>14</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="22">
         <v>70</v>
       </c>
       <c r="D72" t="s">
@@ -2825,13 +2978,13 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="17">
+      <c r="A73" s="16">
         <v>14</v>
       </c>
       <c r="B73">
         <v>1</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="22">
         <v>60</v>
       </c>
       <c r="D73" t="s">
@@ -2845,13 +2998,13 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="17">
+      <c r="A74" s="16">
         <v>14</v>
       </c>
       <c r="B74">
         <v>2</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="22">
         <v>47</v>
       </c>
       <c r="D74" t="s">
@@ -2865,13 +3018,13 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="17">
+      <c r="A75" s="16">
         <v>14</v>
       </c>
       <c r="B75">
         <v>3</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="22">
         <v>40</v>
       </c>
       <c r="D75" t="s">
@@ -2885,14 +3038,14 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="17">
+      <c r="A76" s="16">
         <v>14</v>
       </c>
       <c r="B76">
         <v>4</v>
       </c>
-      <c r="C76">
-        <v>29.37</v>
+      <c r="C76" s="22" t="s">
+        <v>163</v>
       </c>
       <c r="D76" t="s">
         <v>103</v>
@@ -2905,14 +3058,14 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="18">
+      <c r="A77" s="17">
         <v>15</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
-      <c r="C77">
-        <v>0.1</v>
+      <c r="C77" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D77" t="s">
         <v>110</v>
@@ -2925,14 +3078,14 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="18">
+      <c r="A78" s="17">
         <v>15</v>
       </c>
       <c r="B78">
         <v>1</v>
       </c>
-      <c r="C78">
-        <v>0.1</v>
+      <c r="C78" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D78" t="s">
         <v>110</v>
@@ -2945,14 +3098,14 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="18">
+      <c r="A79" s="17">
         <v>15</v>
       </c>
       <c r="B79">
         <v>2</v>
       </c>
-      <c r="C79">
-        <v>0.1</v>
+      <c r="C79" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D79" t="s">
         <v>110</v>
@@ -2965,14 +3118,14 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="18">
+      <c r="A80" s="17">
         <v>15</v>
       </c>
       <c r="B80">
         <v>3</v>
       </c>
-      <c r="C80">
-        <v>0.9</v>
+      <c r="C80" s="22" t="s">
+        <v>127</v>
       </c>
       <c r="D80" t="s">
         <v>110</v>
@@ -2985,14 +3138,14 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="18">
+      <c r="A81" s="17">
         <v>15</v>
       </c>
       <c r="B81">
         <v>4</v>
       </c>
-      <c r="C81">
-        <v>0.9</v>
+      <c r="C81" s="22" t="s">
+        <v>127</v>
       </c>
       <c r="D81" t="s">
         <v>110</v>
@@ -3005,14 +3158,14 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="19">
+      <c r="A82" s="18">
         <v>16</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
-      <c r="C82">
-        <v>0.25</v>
+      <c r="C82" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D82" t="s">
         <v>111</v>
@@ -3025,14 +3178,14 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="19">
+      <c r="A83" s="18">
         <v>16</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
-      <c r="C83">
-        <v>0.25</v>
+      <c r="C83" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D83" t="s">
         <v>111</v>
@@ -3045,14 +3198,14 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="19">
+      <c r="A84" s="18">
         <v>16</v>
       </c>
       <c r="B84">
         <v>2</v>
       </c>
-      <c r="C84">
-        <v>0.25</v>
+      <c r="C84" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D84" t="s">
         <v>111</v>
@@ -3065,14 +3218,14 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="19">
+      <c r="A85" s="18">
         <v>16</v>
       </c>
       <c r="B85">
         <v>3</v>
       </c>
-      <c r="C85">
-        <v>0.25</v>
+      <c r="C85" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D85" t="s">
         <v>111</v>
@@ -3085,14 +3238,14 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="19">
+      <c r="A86" s="18">
         <v>16</v>
       </c>
       <c r="B86">
         <v>4</v>
       </c>
-      <c r="C86">
-        <v>0.25</v>
+      <c r="C86" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D86" t="s">
         <v>111</v>
@@ -3105,14 +3258,14 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="20">
+      <c r="A87" s="19">
         <v>17</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
-      <c r="C87">
-        <v>0.21</v>
+      <c r="C87" s="22" t="s">
+        <v>165</v>
       </c>
       <c r="D87" t="s">
         <v>111</v>
@@ -3125,14 +3278,14 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="20">
+      <c r="A88" s="19">
         <v>17</v>
       </c>
       <c r="B88">
         <v>1</v>
       </c>
-      <c r="C88">
-        <v>0.21</v>
+      <c r="C88" s="22" t="s">
+        <v>165</v>
       </c>
       <c r="D88" t="s">
         <v>111</v>
@@ -3145,14 +3298,14 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="20">
+      <c r="A89" s="19">
         <v>17</v>
       </c>
       <c r="B89">
         <v>2</v>
       </c>
-      <c r="C89">
-        <v>0.21</v>
+      <c r="C89" s="22" t="s">
+        <v>165</v>
       </c>
       <c r="D89" t="s">
         <v>111</v>
@@ -3165,14 +3318,14 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="20">
+      <c r="A90" s="19">
         <v>17</v>
       </c>
       <c r="B90">
         <v>3</v>
       </c>
-      <c r="C90">
-        <v>0.2</v>
+      <c r="C90" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="D90" t="s">
         <v>111</v>
@@ -3185,14 +3338,14 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="20">
+      <c r="A91" s="19">
         <v>17</v>
       </c>
       <c r="B91">
         <v>4</v>
       </c>
-      <c r="C91">
-        <v>0.2</v>
+      <c r="C91" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="D91" t="s">
         <v>111</v>
@@ -3205,14 +3358,14 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="21">
+      <c r="A92" s="20">
         <v>18</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
-      <c r="C92">
-        <v>0.25</v>
+      <c r="C92" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D92" t="s">
         <v>112</v>
@@ -3225,14 +3378,14 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="21">
+      <c r="A93" s="20">
         <v>18</v>
       </c>
       <c r="B93">
         <v>1</v>
       </c>
-      <c r="C93">
-        <v>0.25</v>
+      <c r="C93" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D93" t="s">
         <v>112</v>
@@ -3245,14 +3398,14 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="21">
+      <c r="A94" s="20">
         <v>18</v>
       </c>
       <c r="B94">
         <v>2</v>
       </c>
-      <c r="C94">
-        <v>0.25</v>
+      <c r="C94" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D94" t="s">
         <v>112</v>
@@ -3265,14 +3418,14 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="21">
+      <c r="A95" s="20">
         <v>18</v>
       </c>
       <c r="B95">
         <v>3</v>
       </c>
-      <c r="C95">
-        <v>0.25</v>
+      <c r="C95" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D95" t="s">
         <v>112</v>
@@ -3285,14 +3438,14 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="21">
+      <c r="A96" s="20">
         <v>18</v>
       </c>
       <c r="B96">
         <v>4</v>
       </c>
-      <c r="C96">
-        <v>0.25</v>
+      <c r="C96" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="D96" t="s">
         <v>112</v>
@@ -3305,14 +3458,14 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="22">
+      <c r="A97" s="21">
         <v>19</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
-      <c r="C97">
-        <v>0.88</v>
+      <c r="C97" s="22" t="s">
+        <v>166</v>
       </c>
       <c r="D97" t="s">
         <v>101</v>
@@ -3325,14 +3478,14 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="22">
+      <c r="A98" s="21">
         <v>19</v>
       </c>
       <c r="B98">
         <v>1</v>
       </c>
-      <c r="C98">
-        <v>0.88</v>
+      <c r="C98" s="22" t="s">
+        <v>166</v>
       </c>
       <c r="D98" t="s">
         <v>101</v>
@@ -3345,14 +3498,14 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="22">
+      <c r="A99" s="21">
         <v>19</v>
       </c>
       <c r="B99">
         <v>2</v>
       </c>
-      <c r="C99">
-        <v>0.88</v>
+      <c r="C99" s="22" t="s">
+        <v>166</v>
       </c>
       <c r="D99" t="s">
         <v>101</v>
@@ -3365,14 +3518,14 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="22">
+      <c r="A100" s="21">
         <v>19</v>
       </c>
       <c r="B100">
         <v>3</v>
       </c>
-      <c r="C100">
-        <v>0.88</v>
+      <c r="C100" s="22" t="s">
+        <v>166</v>
       </c>
       <c r="D100" t="s">
         <v>101</v>
@@ -3385,14 +3538,14 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="22">
+      <c r="A101" s="21">
         <v>19</v>
       </c>
       <c r="B101">
         <v>4</v>
       </c>
-      <c r="C101">
-        <v>0.88</v>
+      <c r="C101" s="22" t="s">
+        <v>166</v>
       </c>
       <c r="D101" t="s">
         <v>101</v>
@@ -3435,7 +3588,9 @@
     <hyperlink ref="F47" r:id="rId27" xr:uid="{D8E511FF-DC35-47E0-863D-EBF7A6FF4802}"/>
     <hyperlink ref="F48" r:id="rId28" xr:uid="{DAACB6E2-9A25-462C-85A1-5AAD01B90A5A}"/>
     <hyperlink ref="F51" r:id="rId29" xr:uid="{38C6F7F3-40DE-4A43-BDDE-E296D4015F89}"/>
+    <hyperlink ref="F67" r:id="rId30" xr:uid="{E8F9291B-5C61-4A97-AB97-43FD0AFEDB0A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>